<commit_message>
Full Update to repo from MacLap
</commit_message>
<xml_diff>
--- a/_Radial_Velocity_Data/Annika_Results_List_1/Overview.xlsx
+++ b/_Radial_Velocity_Data/Annika_Results_List_1/Overview.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830C611B-A353-C84E-8B9A-FA42BE67B027}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C00EBC0-B132-6240-B54C-475121E9AB75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="480" windowWidth="21960" windowHeight="8680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annika_List_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -229,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -355,6 +361,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -710,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -744,10 +757,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -764,8 +777,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
@@ -780,12 +793,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -794,8 +807,8 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="2" t="s">
         <v>36</v>
       </c>
@@ -813,13 +826,13 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -846,10 +859,10 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -864,8 +877,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
@@ -881,7 +894,7 @@
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="12" t="s">
@@ -910,10 +923,10 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -930,8 +943,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="11" t="s">
         <v>53</v>
       </c>
@@ -991,7 +1004,7 @@
       <c r="C18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1009,7 +1022,7 @@
       <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="1"/>
@@ -1040,10 +1053,10 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1060,8 +1073,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1125,8 +1138,12 @@
     <hyperlink ref="D14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="D24" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D23" r:id="rId6" xr:uid="{473A5CAB-7F64-6545-8824-5690DC80E108}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{7C77F5D3-9F54-8E44-8788-32FD7C9D7DA8}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{3A02BC16-86C7-6E48-B519-C75ECD134D49}"/>
+    <hyperlink ref="D18" r:id="rId9" xr:uid="{0C48FABF-538C-9342-AC90-742B3E01F054}"/>
+    <hyperlink ref="D19" r:id="rId10" location="/browse" xr:uid="{3764052D-930A-C14B-BDC3-468700B26F97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>